<commit_message>
Improve PRF email HTML, tidy, tidy PRF template
</commit_message>
<xml_diff>
--- a/services/dsrp-api/app/templates/payment_request_form.xlsx
+++ b/services/dsrp-api/app/templates/payment_request_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\source\repos\dormant-site-reclamation-program\services\dsrp-api\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B273E461-1EC3-495F-A4C0-38DC8B27AF14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD807AC-8F56-4CA9-A365-AC272FB37E34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5150" yWindow="4790" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Program</t>
   </si>
@@ -69,12 +69,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Special Instructions</t>
-  </si>
-  <si>
     <t>Total Payment</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>{d.po_number}</t>
   </si>
   <si>
-    <t>{d.special_instructions}</t>
-  </si>
-  <si>
     <t>{d.qualified_receiver_name}</t>
   </si>
   <si>
@@ -118,12 +109,6 @@
   </si>
   <si>
     <t>{d.payment_details[i+1].amount}</t>
-  </si>
-  <si>
-    <t>{d.payment_details[i].comments}</t>
-  </si>
-  <si>
-    <t>{d.payment_details[i+1].comments}</t>
   </si>
   <si>
     <t>{d.total_payment}</t>
@@ -176,10 +161,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -461,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,189 +462,169 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
+  <mergeCells count="9">
     <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B13:E13"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Move "Total Amount" in PRF template, edit PRF HTML email styling
</commit_message>
<xml_diff>
--- a/services/dsrp-api/app/templates/payment_request_form.xlsx
+++ b/services/dsrp-api/app/templates/payment_request_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\source\repos\dormant-site-reclamation-program\services\dsrp-api\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD807AC-8F56-4CA9-A365-AC272FB37E34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAE661B-D4A3-4046-8B4A-7E0237DBB02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5150" yWindow="4790" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4180" yWindow="4180" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Total Payment</t>
-  </si>
-  <si>
     <t>{d.supplier_name}</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>{d.account_coding}</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B10" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,7 +474,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -485,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -496,7 +496,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -507,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -530,44 +530,44 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -575,7 +575,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -586,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -597,7 +597,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -608,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>

</xml_diff>

<commit_message>
Add Invoice Date field to PRF
</commit_message>
<xml_diff>
--- a/services/dsrp-api/app/templates/payment_request_form.xlsx
+++ b/services/dsrp-api/app/templates/payment_request_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\source\repos\dormant-site-reclamation-program\services\dsrp-api\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAE661B-D4A3-4046-8B4A-7E0237DBB02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEB2F05-AA60-41B0-986B-62F1817FB003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="4180" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4520" yWindow="4530" windowWidth="28780" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Program</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Total Amount</t>
+  </si>
+  <si>
+    <t>Invoice Date</t>
+  </si>
+  <si>
+    <t>{d.invoice_date}</t>
   </si>
 </sst>
 </file>
@@ -161,10 +167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -447,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -462,168 +469,172 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B10:E10"/>
+  <mergeCells count="8">
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update company payment info QR name, update PRF email subject line
</commit_message>
<xml_diff>
--- a/services/dsrp-api/app/templates/payment_request_form.xlsx
+++ b/services/dsrp-api/app/templates/payment_request_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\source\repos\dormant-site-reclamation-program\services\dsrp-api\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEB2F05-AA60-41B0-986B-62F1817FB003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636D0028-A83E-45E4-A802-3B1EC04ACAAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="4530" windowWidth="28780" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Account Coding</t>
   </si>
   <si>
-    <t>Qualified Receiver Name</t>
-  </si>
-  <si>
     <t>Date Payment Authorized</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>{d.invoice_date}</t>
+  </si>
+  <si>
+    <t>Qualified Receiver Names</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,7 +481,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -492,7 +492,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -503,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -511,10 +511,10 @@
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -522,72 +522,72 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -595,10 +595,10 @@
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -606,10 +606,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -620,7 +620,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>

</xml_diff>

<commit_message>
Combine two resource files (payment document), use association table for payment documents m:m with contracted work, fix issue with PRF template,
</commit_message>
<xml_diff>
--- a/services/dsrp-api/app/templates/payment_request_form.xlsx
+++ b/services/dsrp-api/app/templates/payment_request_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\source\repos\dormant-site-reclamation-program\services\dsrp-api\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636D0028-A83E-45E4-A802-3B1EC04ACAAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0364AC-0016-4AEA-A04A-DDB58BFCA91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3500" windowWidth="28780" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,130 +509,134 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="D15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B10:E10"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Put WANs in PRFs
</commit_message>
<xml_diff>
--- a/services/dsrp-api/app/templates/payment_request_form.xlsx
+++ b/services/dsrp-api/app/templates/payment_request_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\source\repos\dormant-site-reclamation-program\services\dsrp-api\app\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\source\repos\bcgov\dormant-site-reclamation-program\services\dsrp-api\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0364AC-0016-4AEA-A04A-DDB58BFCA91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14091F59-4074-4558-AD6E-FDBA580229BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3500" windowWidth="28780" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3800" yWindow="3800" windowWidth="28780" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Program</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>Qualified Receiver Names</t>
+  </si>
+  <si>
+    <t>Well Authorization Number</t>
+  </si>
+  <si>
+    <t>{d.payment_details[i].well_authorization_number}</t>
+  </si>
+  <si>
+    <t>{d.payment_details[i+1].well_authorization_number}</t>
   </si>
 </sst>
 </file>
@@ -457,7 +466,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -580,9 +589,11 @@
         <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -595,6 +606,9 @@
         <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -609,6 +623,9 @@
         <v>23</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -622,7 +639,10 @@
       <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>